<commit_message>
a lot of bug
</commit_message>
<xml_diff>
--- a/Stat reports/Reports/Templates/1-ис (инвестиции).xlsx
+++ b/Stat reports/Reports/Templates/1-ис (инвестиции).xlsx
@@ -3,14 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Статотчетность_дирекция\templates\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB2E6BA-956D-4682-8DAE-919355C0D597}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21375" windowHeight="7905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="21375" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="Главная" sheetId="1" r:id="rId1"/>
@@ -28,32 +22,32 @@
     <sheet name="Раздел 12" sheetId="13" r:id="rId13"/>
     <sheet name="Раздел 13" sheetId="14" r:id="rId14"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="314">
   <si>
-    <t>ГОСУДАРСТВЕННАЯ СТАТИСТИЧЕСКАЯ ОТЧЕТНОСТЬ</t>
-  </si>
-  <si>
-    <t>КОНФИДЕНЦИАЛЬНОСТЬ ГАРАНТИРУЕТСЯ ПОЛУЧАТЕЛЕМ ИНФОРМАЦИИ</t>
-  </si>
-  <si>
-    <t>Представление искаженных данных государственной статистической отчетности, несвоевременное представление или непредставление такой отчетности влекут применение мер административной или уголовной ответственности в порядке, установленном законодательством Республики Беларусь</t>
-  </si>
-  <si>
-    <t>Представляют респонденты</t>
-  </si>
-  <si>
-    <t>Срок представления</t>
-  </si>
-  <si>
-    <t>1-ис (инвестиции)</t>
-  </si>
-  <si>
-    <t>Юридические лица (кроме перечисленных в Указаниях по
+    <t xml:space="preserve">ГОСУДАРСТВЕННАЯ СТАТИСТИЧЕСКАЯ ОТЧЕТНОСТЬ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">КОНФИДЕНЦИАЛЬНОСТЬ ГАРАНТИРУЕТСЯ ПОЛУЧАТЕЛЕМ ИНФОРМАЦИИ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Представление искаженных данных государственной статистической отчетности, несвоевременное представление или непредставление такой отчетности влекут применение мер административной или уголовной ответственности в порядке, установленном законодательством Республики Беларусь</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Представляют респонденты</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Срок представления</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-ис (инвестиции)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Юридические лица (кроме перечисленных в Указаниях по
 заполнению настоящей формы), обособленные подразделения
 юридических лиц, осуществляющие инвестиционную деятельность
 по вложению инвестиций в основной капитал.
@@ -66,106 +60,106 @@
 управление области.</t>
   </si>
   <si>
-    <t>27 февраля</t>
-  </si>
-  <si>
-    <t>Код формы
+    <t xml:space="preserve">27 февраля</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Код формы
 по ОКУД</t>
   </si>
   <si>
-    <t>0628004</t>
-  </si>
-  <si>
-    <t>Годовая</t>
-  </si>
-  <si>
-    <t>Полное наименование юридического лица: ОТКРЫТОЕ АКЦИОНЕРНОЕ ОБЩЕСТВО "СТРОЙТРЕСТ N 3 ОРДЕНА
+    <t xml:space="preserve">0628004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Годовая</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Полное наименование юридического лица: ОТКРЫТОЕ АКЦИОНЕРНОЕ ОБЩЕСТВО "СТРОЙТРЕСТ N 3 ОРДЕНА
 ОКТЯБРЬСКОЙ РЕВОЛЮЦИИ"</t>
   </si>
   <si>
-    <t>Полное наименование обособленного подразделения юридического лица: СТРОИТЕЛЬНОЕ УПРАВЛЕНИЕ N 149
+    <t xml:space="preserve">Полное наименование обособленного подразделения юридического лица: СТРОИТЕЛЬНОЕ УПРАВЛЕНИЕ N 149
 ОТКРЫТОГО АКЦИОНЕРНОГО ОБЩЕСТВА "СТРОЙТРЕСТ N 3 ОРДЕНА ОКТЯБРЬСКОЙ РЕВОЛЮЦИИ"</t>
   </si>
   <si>
-    <t>Местоположение: 223710, МИНСКАЯ ОБЛАСТЬ, Солигорский, Солигорск, УЛ. КОЗЛОВА, 37</t>
-  </si>
-  <si>
-    <t>Электронный адрес: su149@str3.by</t>
-  </si>
-  <si>
-    <t>Регистрационный номер в статистическом регистре (ОКПО)</t>
-  </si>
-  <si>
-    <t>Учетный номер плательщика (УНП)</t>
-  </si>
-  <si>
-    <t>Территория нахождения объекта инвестиционной деятельности</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>012774946009</t>
-  </si>
-  <si>
-    <t>600142668</t>
-  </si>
-  <si>
-    <t>Солигорский район</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>Мощность объектов:</t>
-  </si>
-  <si>
-    <t>В</t>
-  </si>
-  <si>
-    <t>Б</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>реконструкции,
+    <t xml:space="preserve">Местоположение: 223710, МИНСКАЯ ОБЛАСТЬ, Солигорский, Солигорск, УЛ. КОЗЛОВА, 37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Электронный адрес: su149@str3.by</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Регистрационный номер в статистическом регистре (ОКПО)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Учетный номер плательщика (УНП)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Территория нахождения объекта инвестиционной деятельности</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">012774946009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">600142668</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Солигорский район</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Мощность объектов:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">В</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Б</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">реконструкции,
 модернизации</t>
   </si>
   <si>
-    <t>возведения</t>
-  </si>
-  <si>
-    <t>Из них в результате</t>
-  </si>
-  <si>
-    <t>Введено
+    <t xml:space="preserve">возведения</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Из них в результате</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Введено
 в
 эксплуатацию</t>
   </si>
   <si>
-    <t>Ед.измерения</t>
-  </si>
-  <si>
-    <t>Код</t>
-  </si>
-  <si>
-    <t>Наименование показателя</t>
-  </si>
-  <si>
-    <t>Раздел 1</t>
-  </si>
-  <si>
-    <t>Ввод в эксплуатацию объектов строительства</t>
+    <t xml:space="preserve">Ед.измерения</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Код</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Наименование показателя</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Раздел 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ввод в эксплуатацию объектов строительства</t>
   </si>
   <si>
     <t xml:space="preserve">Таблица 1  </t>
@@ -174,353 +168,353 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>111</t>
-  </si>
-  <si>
-    <t>других зданий</t>
-  </si>
-  <si>
-    <t>110</t>
-  </si>
-  <si>
-    <t>административных</t>
-  </si>
-  <si>
-    <t>106</t>
-  </si>
-  <si>
-    <t>здравоохранения</t>
-  </si>
-  <si>
-    <t>105</t>
-  </si>
-  <si>
-    <t>учебных</t>
-  </si>
-  <si>
-    <t>104</t>
-  </si>
-  <si>
-    <t>коммерческих</t>
-  </si>
-  <si>
-    <t>103</t>
-  </si>
-  <si>
-    <t>сельскохозяйственных</t>
-  </si>
-  <si>
-    <t>102</t>
-  </si>
-  <si>
-    <t>в том числе: промышленных</t>
-  </si>
-  <si>
-    <t>101</t>
-  </si>
-  <si>
-    <t>Введено в эксплуатацию новых нежилых зданий (сумма строк с 102 по 106, 110 и
+    <t xml:space="preserve">111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">других зданий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">административных</t>
+  </si>
+  <si>
+    <t xml:space="preserve">106</t>
+  </si>
+  <si>
+    <t xml:space="preserve">здравоохранения</t>
+  </si>
+  <si>
+    <t xml:space="preserve">105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">учебных</t>
+  </si>
+  <si>
+    <t xml:space="preserve">104</t>
+  </si>
+  <si>
+    <t xml:space="preserve">коммерческих</t>
+  </si>
+  <si>
+    <t xml:space="preserve">103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">сельскохозяйственных</t>
+  </si>
+  <si>
+    <t xml:space="preserve">102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">в том числе: промышленных</t>
+  </si>
+  <si>
+    <t xml:space="preserve">101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Введено в эксплуатацию новых нежилых зданий (сумма строк с 102 по 106, 110 и
 111)</t>
   </si>
   <si>
-    <t>Количество,
+    <t xml:space="preserve">Количество,
 единиц</t>
   </si>
   <si>
-    <t>Раздел 2</t>
-  </si>
-  <si>
-    <t>Ввод в эксплуатацию новых нежилых зданий</t>
+    <t xml:space="preserve">Раздел 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ввод в эксплуатацию новых нежилых зданий</t>
   </si>
   <si>
     <t xml:space="preserve">Таблица 2  </t>
   </si>
   <si>
-    <t>Общая
+    <t xml:space="preserve">Общая
 площадь,
 квадратных
 метров</t>
   </si>
   <si>
-    <t>Фактическая
+    <t xml:space="preserve">Фактическая
 стоимость,
 тысяч
 рублей</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>240</t>
-  </si>
-  <si>
-    <t>техника вычислительная и организационная</t>
-  </si>
-  <si>
-    <t>238</t>
-  </si>
-  <si>
-    <t>транспортные средства</t>
-  </si>
-  <si>
-    <t>237</t>
-  </si>
-  <si>
-    <t>финансовый лизинг</t>
-  </si>
-  <si>
-    <t>236</t>
-  </si>
-  <si>
-    <t>Из строки 222: работы по монтажу оборудования</t>
-  </si>
-  <si>
-    <t>235</t>
-  </si>
-  <si>
-    <t>автомобильные дороги необщего пользования</t>
-  </si>
-  <si>
-    <t>234</t>
-  </si>
-  <si>
-    <t>автомобильные дороги общего пользования</t>
-  </si>
-  <si>
-    <t>233</t>
-  </si>
-  <si>
-    <t>эксплуатационное бурение на нефть и газ</t>
-  </si>
-  <si>
-    <t>232</t>
-  </si>
-  <si>
-    <t>глубокое разведочное бурение на нефть и газ</t>
-  </si>
-  <si>
-    <t>231</t>
-  </si>
-  <si>
-    <t>закладка садов и других многолетних насаждений</t>
-  </si>
-  <si>
-    <t>230</t>
-  </si>
-  <si>
-    <t>мелиорация земель</t>
-  </si>
-  <si>
-    <t>239</t>
-  </si>
-  <si>
-    <t>из них сооружения и передаточные устройства</t>
-  </si>
-  <si>
-    <t>228</t>
-  </si>
-  <si>
-    <t>Из строки 202: здания (кроме жилых), сооружения и передаточные устройства</t>
-  </si>
-  <si>
-    <t>248</t>
-  </si>
-  <si>
-    <t>разведка и оценка запасов полезных ископаемых</t>
-  </si>
-  <si>
-    <t>247</t>
-  </si>
-  <si>
-    <t>оригиналы произведений развлекательного жанра, литературы или искусства</t>
-  </si>
-  <si>
-    <t>519</t>
-  </si>
-  <si>
-    <t>246</t>
-  </si>
-  <si>
-    <t>научные исследования и разработки</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>245</t>
-  </si>
-  <si>
-    <t>из них: программное обеспечение и базы данных</t>
-  </si>
-  <si>
-    <t>529</t>
-  </si>
-  <si>
-    <t>244</t>
-  </si>
-  <si>
-    <t>объекты интеллектуальной собственности</t>
-  </si>
-  <si>
-    <t>227</t>
-  </si>
-  <si>
-    <t>из них для строительства будущих лет</t>
-  </si>
-  <si>
-    <t>226</t>
-  </si>
-  <si>
-    <t>из них проектно-изыскательские работы</t>
-  </si>
-  <si>
-    <t>225</t>
-  </si>
-  <si>
-    <t>прочие работы и затраты</t>
-  </si>
-  <si>
-    <t>223</t>
-  </si>
-  <si>
-    <t>из них импортные</t>
-  </si>
-  <si>
-    <t>222</t>
-  </si>
-  <si>
-    <t>машины, оборудование, транспортные средства, инструмент, инвентарь</t>
-  </si>
-  <si>
-    <t>220</t>
-  </si>
-  <si>
-    <t>в том числе: строительно-монтажные работы</t>
-  </si>
-  <si>
-    <t>202</t>
-  </si>
-  <si>
-    <t>Использовано инвестиций в основной капитал - всего (сумма строк 220, 222, 225,
+    <t xml:space="preserve">11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">240</t>
+  </si>
+  <si>
+    <t xml:space="preserve">техника вычислительная и организационная</t>
+  </si>
+  <si>
+    <t xml:space="preserve">238</t>
+  </si>
+  <si>
+    <t xml:space="preserve">транспортные средства</t>
+  </si>
+  <si>
+    <t xml:space="preserve">237</t>
+  </si>
+  <si>
+    <t xml:space="preserve">финансовый лизинг</t>
+  </si>
+  <si>
+    <t xml:space="preserve">236</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Из строки 222: работы по монтажу оборудования</t>
+  </si>
+  <si>
+    <t xml:space="preserve">235</t>
+  </si>
+  <si>
+    <t xml:space="preserve">автомобильные дороги необщего пользования</t>
+  </si>
+  <si>
+    <t xml:space="preserve">234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">автомобильные дороги общего пользования</t>
+  </si>
+  <si>
+    <t xml:space="preserve">233</t>
+  </si>
+  <si>
+    <t xml:space="preserve">эксплуатационное бурение на нефть и газ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">232</t>
+  </si>
+  <si>
+    <t xml:space="preserve">глубокое разведочное бурение на нефть и газ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">231</t>
+  </si>
+  <si>
+    <t xml:space="preserve">закладка садов и других многолетних насаждений</t>
+  </si>
+  <si>
+    <t xml:space="preserve">230</t>
+  </si>
+  <si>
+    <t xml:space="preserve">мелиорация земель</t>
+  </si>
+  <si>
+    <t xml:space="preserve">239</t>
+  </si>
+  <si>
+    <t xml:space="preserve">из них сооружения и передаточные устройства</t>
+  </si>
+  <si>
+    <t xml:space="preserve">228</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Из строки 202: здания (кроме жилых), сооружения и передаточные устройства</t>
+  </si>
+  <si>
+    <t xml:space="preserve">248</t>
+  </si>
+  <si>
+    <t xml:space="preserve">разведка и оценка запасов полезных ископаемых</t>
+  </si>
+  <si>
+    <t xml:space="preserve">247</t>
+  </si>
+  <si>
+    <t xml:space="preserve">оригиналы произведений развлекательного жанра, литературы или искусства</t>
+  </si>
+  <si>
+    <t xml:space="preserve">519</t>
+  </si>
+  <si>
+    <t xml:space="preserve">246</t>
+  </si>
+  <si>
+    <t xml:space="preserve">научные исследования и разработки</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">245</t>
+  </si>
+  <si>
+    <t xml:space="preserve">из них: программное обеспечение и базы данных</t>
+  </si>
+  <si>
+    <t xml:space="preserve">529</t>
+  </si>
+  <si>
+    <t xml:space="preserve">244</t>
+  </si>
+  <si>
+    <t xml:space="preserve">объекты интеллектуальной собственности</t>
+  </si>
+  <si>
+    <t xml:space="preserve">227</t>
+  </si>
+  <si>
+    <t xml:space="preserve">из них для строительства будущих лет</t>
+  </si>
+  <si>
+    <t xml:space="preserve">226</t>
+  </si>
+  <si>
+    <t xml:space="preserve">из них проектно-изыскательские работы</t>
+  </si>
+  <si>
+    <t xml:space="preserve">225</t>
+  </si>
+  <si>
+    <t xml:space="preserve">прочие работы и затраты</t>
+  </si>
+  <si>
+    <t xml:space="preserve">223</t>
+  </si>
+  <si>
+    <t xml:space="preserve">из них импортные</t>
+  </si>
+  <si>
+    <t xml:space="preserve">222</t>
+  </si>
+  <si>
+    <t xml:space="preserve">машины, оборудование, транспортные средства, инструмент, инвентарь</t>
+  </si>
+  <si>
+    <t xml:space="preserve">220</t>
+  </si>
+  <si>
+    <t xml:space="preserve">в том числе: строительно-монтажные работы</t>
+  </si>
+  <si>
+    <t xml:space="preserve">202</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Использовано инвестиций в основной капитал - всего (сумма строк 220, 222, 225,
 244)</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>из
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">из
 них
 модернизации</t>
   </si>
   <si>
-    <t>Всего</t>
-  </si>
-  <si>
-    <t>Раздел 3</t>
-  </si>
-  <si>
-    <t>Основные средства и инвестиции в основной капитал</t>
-  </si>
-  <si>
-    <t>Таблица 3 Технологическая и воспроизводственная структура инвестиций в основной капитал</t>
-  </si>
-  <si>
-    <t>тысяч рублей</t>
-  </si>
-  <si>
-    <t>243</t>
-  </si>
-  <si>
-    <t>затраты по формированию основного стада</t>
-  </si>
-  <si>
-    <t>242</t>
-  </si>
-  <si>
-    <t>Из строки 202: уплаченные банку проценты по кредитам (займам)</t>
-  </si>
-  <si>
-    <t>241</t>
-  </si>
-  <si>
-    <t>Сумма налога на добавленную стоимость за использованные объемы инвестиций в
+    <t xml:space="preserve">Всего</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Раздел 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Основные средства и инвестиции в основной капитал</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Таблица 3 Технологическая и воспроизводственная структура инвестиций в основной капитал</t>
+  </si>
+  <si>
+    <t xml:space="preserve">тысяч рублей</t>
+  </si>
+  <si>
+    <t xml:space="preserve">243</t>
+  </si>
+  <si>
+    <t xml:space="preserve">затраты по формированию основного стада</t>
+  </si>
+  <si>
+    <t xml:space="preserve">242</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Из строки 202: уплаченные банку проценты по кредитам (займам)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">241</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сумма налога на добавленную стоимость за использованные объемы инвестиций в
 основной капитал</t>
   </si>
   <si>
-    <t>Всего,
+    <t xml:space="preserve">Всего,
 тысяч
 рублей</t>
   </si>
   <si>
-    <t>Таблица 4 Справочная информация</t>
-  </si>
-  <si>
-    <t>41200</t>
-  </si>
-  <si>
-    <t>Общее строительство зданий</t>
-  </si>
-  <si>
-    <t>251</t>
-  </si>
-  <si>
-    <t>в том числе по видам экономической деятельности:</t>
-  </si>
-  <si>
-    <t>250</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>льготных
+    <t xml:space="preserve">Таблица 4 Справочная информация</t>
+  </si>
+  <si>
+    <t xml:space="preserve">41200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Общее строительство зданий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">251</t>
+  </si>
+  <si>
+    <t xml:space="preserve">в том числе по видам экономической деятельности:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">льготных
 кредитов</t>
   </si>
   <si>
-    <t>прочих
+    <t xml:space="preserve">прочих
 источников</t>
   </si>
   <si>
-    <t>средств
+    <t xml:space="preserve">средств
 населения</t>
   </si>
   <si>
-    <t>из них</t>
-  </si>
-  <si>
-    <t>кредитов
+    <t xml:space="preserve">из них</t>
+  </si>
+  <si>
+    <t xml:space="preserve">кредитов
 (займов)
 банков</t>
   </si>
   <si>
-    <t>иностранных
+    <t xml:space="preserve">иностранных
 инвестиций
 (без
 кредитов
@@ -529,22 +523,22 @@
 банков)</t>
   </si>
   <si>
-    <t>средств
+    <t xml:space="preserve">средств
 внебюджетных фондов</t>
   </si>
   <si>
-    <t>средств
+    <t xml:space="preserve">средств
 местных
 бюджетов</t>
   </si>
   <si>
-    <t>заемных
+    <t xml:space="preserve">заемных
 средств
 других
 организаций</t>
   </si>
   <si>
-    <t>из
+    <t xml:space="preserve">из
 них
 за
 счет
@@ -554,28 +548,28 @@
 распределенной</t>
   </si>
   <si>
-    <t>собственных
+    <t xml:space="preserve">собственных
 средств
 организаций</t>
   </si>
   <si>
-    <t>В том числе за счет</t>
-  </si>
-  <si>
-    <t>Наименование вида экономической деятельности по ОКРБ 005-2011</t>
-  </si>
-  <si>
-    <t>Таблица 5 Ввод в эксплуатацию основных средств и использование инвестиций в основной капитал по источникам финансирования и видам экономической деятельности</t>
-  </si>
-  <si>
-    <t>Введено
+    <t xml:space="preserve">В том числе за счет</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Наименование вида экономической деятельности по ОКРБ 005-2011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Таблица 5 Ввод в эксплуатацию основных средств и использование инвестиций в основной капитал по источникам финансирования и видам экономической деятельности</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Введено
 в
 эксплуатацию
 основных
 средств</t>
   </si>
   <si>
-    <t>Использовано
+    <t xml:space="preserve">Использовано
 инвестиций
 в
 основной
@@ -587,25 +581,25 @@
 1)</t>
   </si>
   <si>
-    <t>средств
+    <t xml:space="preserve">средств
 республиканского
 бюджета</t>
   </si>
   <si>
-    <t>кредитов
+    <t xml:space="preserve">кредитов
 (займов)
 иностранных
 банков</t>
   </si>
   <si>
-    <t>кредитов
+    <t xml:space="preserve">кредитов
 по
 иностранным
 кредитным
 линиям</t>
   </si>
   <si>
-    <t>из
+    <t xml:space="preserve">из
 графы
 6
 -
@@ -615,16 +609,16 @@
 займов</t>
   </si>
   <si>
-    <t>351</t>
-  </si>
-  <si>
-    <t>350</t>
-  </si>
-  <si>
-    <t>Таблица 6 Технологическая структура инвестиций в основной капитал по видам экономической деятельности</t>
-  </si>
-  <si>
-    <t>Строительно-монтажные
+    <t xml:space="preserve">351</t>
+  </si>
+  <si>
+    <t xml:space="preserve">350</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Таблица 6 Технологическая структура инвестиций в основной капитал по видам экономической деятельности</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Строительно-монтажные
 работы
 (из
 строки
@@ -633,7 +627,7 @@
 1)</t>
   </si>
   <si>
-    <t>Машины,
+    <t xml:space="preserve">Машины,
 оборудование,
 транспортные
 средства,
@@ -646,7 +640,7 @@
 1)</t>
   </si>
   <si>
-    <t>импортные
+    <t xml:space="preserve">импортные
 (из
 строки
 223
@@ -654,7 +648,7 @@
 1)</t>
   </si>
   <si>
-    <t>работы
+    <t xml:space="preserve">работы
 по
 монтажу
 оборудования
@@ -664,71 +658,71 @@
 1)</t>
   </si>
   <si>
-    <t>409</t>
-  </si>
-  <si>
-    <t>прочую деятельность в области охраны окружающей среды</t>
-  </si>
-  <si>
-    <t>408</t>
-  </si>
-  <si>
-    <t>научную деятельность и разработки в области охраны окружающей среды</t>
-  </si>
-  <si>
-    <t>407</t>
-  </si>
-  <si>
-    <t>защиту от ионизирующего излучения и радиоактивного загрязнения</t>
-  </si>
-  <si>
-    <t>406</t>
-  </si>
-  <si>
-    <t>сохранение биологического и ландшафтного разнообразия</t>
-  </si>
-  <si>
-    <t>405</t>
-  </si>
-  <si>
-    <t>снижение шумового и вибрационного воздействия</t>
-  </si>
-  <si>
-    <t>404</t>
-  </si>
-  <si>
-    <t>охрану и экологическую реабилитацию земель, поверхностных и подземных вод</t>
-  </si>
-  <si>
-    <t>403</t>
-  </si>
-  <si>
-    <t>обращение с отходами</t>
-  </si>
-  <si>
-    <t>402</t>
-  </si>
-  <si>
-    <t>обращение со сточными водами</t>
-  </si>
-  <si>
-    <t>401</t>
-  </si>
-  <si>
-    <t>в том числе на: охрану атмосферного воздуха и предотвращение изменения климата</t>
-  </si>
-  <si>
-    <t>400</t>
-  </si>
-  <si>
-    <t>иных
+    <t xml:space="preserve">409</t>
+  </si>
+  <si>
+    <t xml:space="preserve">прочую деятельность в области охраны окружающей среды</t>
+  </si>
+  <si>
+    <t xml:space="preserve">408</t>
+  </si>
+  <si>
+    <t xml:space="preserve">научную деятельность и разработки в области охраны окружающей среды</t>
+  </si>
+  <si>
+    <t xml:space="preserve">407</t>
+  </si>
+  <si>
+    <t xml:space="preserve">защиту от ионизирующего излучения и радиоактивного загрязнения</t>
+  </si>
+  <si>
+    <t xml:space="preserve">406</t>
+  </si>
+  <si>
+    <t xml:space="preserve">сохранение биологического и ландшафтного разнообразия</t>
+  </si>
+  <si>
+    <t xml:space="preserve">405</t>
+  </si>
+  <si>
+    <t xml:space="preserve">снижение шумового и вибрационного воздействия</t>
+  </si>
+  <si>
+    <t xml:space="preserve">404</t>
+  </si>
+  <si>
+    <t xml:space="preserve">охрану и экологическую реабилитацию земель, поверхностных и подземных вод</t>
+  </si>
+  <si>
+    <t xml:space="preserve">403</t>
+  </si>
+  <si>
+    <t xml:space="preserve">обращение с отходами</t>
+  </si>
+  <si>
+    <t xml:space="preserve">402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">обращение со сточными водами</t>
+  </si>
+  <si>
+    <t xml:space="preserve">401</t>
+  </si>
+  <si>
+    <t xml:space="preserve">в том числе на: охрану атмосферного воздуха и предотвращение изменения климата</t>
+  </si>
+  <si>
+    <t xml:space="preserve">400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">иных
 источников</t>
   </si>
   <si>
-    <t>Таблица 7 Инвестиции в основной капитал, направленные на охрану окружающей среды</t>
-  </si>
-  <si>
-    <t>Использовано
+    <t xml:space="preserve">Таблица 7 Инвестиции в основной капитал, направленные на охрану окружающей среды</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Использовано
 инвестиций
 в
 основной
@@ -743,10 +737,10 @@
 по 6)</t>
   </si>
   <si>
-    <t>500</t>
-  </si>
-  <si>
-    <t>Из
+    <t xml:space="preserve">500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Из
 них
 в
 сельских
@@ -754,97 +748,97 @@
 пунктах</t>
   </si>
   <si>
-    <t>Раздел 4</t>
-  </si>
-  <si>
-    <t>Строительство объектов жилищно-гражданского назначения</t>
-  </si>
-  <si>
-    <t>Таблица 8 Строительство объектов социально-культурного назначения</t>
-  </si>
-  <si>
-    <t>прочих источников</t>
-  </si>
-  <si>
-    <t>518</t>
-  </si>
-  <si>
-    <t>средств населения</t>
-  </si>
-  <si>
-    <t>517</t>
-  </si>
-  <si>
-    <t>из них льготных кредитов</t>
-  </si>
-  <si>
-    <t>516</t>
-  </si>
-  <si>
-    <t>кредитов (займов) банков</t>
-  </si>
-  <si>
-    <t>515</t>
-  </si>
-  <si>
-    <t>иностранных инвестиций (без кредитов (займов) иностранных банков)</t>
-  </si>
-  <si>
-    <t>514</t>
-  </si>
-  <si>
-    <t>средств внебюджетных фондов</t>
-  </si>
-  <si>
-    <t>513</t>
-  </si>
-  <si>
-    <t>средств местных бюджетов</t>
-  </si>
-  <si>
-    <t>520</t>
-  </si>
-  <si>
-    <t>из них средств семейного капитала</t>
-  </si>
-  <si>
-    <t>512</t>
-  </si>
-  <si>
-    <t>средств республиканского бюджета</t>
-  </si>
-  <si>
-    <t>511</t>
-  </si>
-  <si>
-    <t>заемных средств других организаций</t>
-  </si>
-  <si>
-    <t>510</t>
-  </si>
-  <si>
-    <t>Из строки 502 - за счет: собственных средств организаций</t>
-  </si>
-  <si>
-    <t>508</t>
-  </si>
-  <si>
-    <t>Из строки 502: в малых городских поселениях</t>
-  </si>
-  <si>
-    <t>503</t>
-  </si>
-  <si>
-    <t>из них общежития</t>
-  </si>
-  <si>
-    <t>502</t>
-  </si>
-  <si>
-    <t>Жилые дома и общежития (сумма строк с 510 по 516, 518, 519)</t>
-  </si>
-  <si>
-    <t>Использовано
+    <t xml:space="preserve">Раздел 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Строительство объектов жилищно-гражданского назначения</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Таблица 8 Строительство объектов социально-культурного назначения</t>
+  </si>
+  <si>
+    <t xml:space="preserve">прочих источников</t>
+  </si>
+  <si>
+    <t xml:space="preserve">518</t>
+  </si>
+  <si>
+    <t xml:space="preserve">средств населения</t>
+  </si>
+  <si>
+    <t xml:space="preserve">517</t>
+  </si>
+  <si>
+    <t xml:space="preserve">из них льготных кредитов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">516</t>
+  </si>
+  <si>
+    <t xml:space="preserve">кредитов (займов) банков</t>
+  </si>
+  <si>
+    <t xml:space="preserve">515</t>
+  </si>
+  <si>
+    <t xml:space="preserve">иностранных инвестиций (без кредитов (займов) иностранных банков)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">514</t>
+  </si>
+  <si>
+    <t xml:space="preserve">средств внебюджетных фондов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">513</t>
+  </si>
+  <si>
+    <t xml:space="preserve">средств местных бюджетов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">520</t>
+  </si>
+  <si>
+    <t xml:space="preserve">из них средств семейного капитала</t>
+  </si>
+  <si>
+    <t xml:space="preserve">512</t>
+  </si>
+  <si>
+    <t xml:space="preserve">средств республиканского бюджета</t>
+  </si>
+  <si>
+    <t xml:space="preserve">511</t>
+  </si>
+  <si>
+    <t xml:space="preserve">заемных средств других организаций</t>
+  </si>
+  <si>
+    <t xml:space="preserve">510</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Из строки 502 - за счет: собственных средств организаций</t>
+  </si>
+  <si>
+    <t xml:space="preserve">508</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Из строки 502: в малых городских поселениях</t>
+  </si>
+  <si>
+    <t xml:space="preserve">503</t>
+  </si>
+  <si>
+    <t xml:space="preserve">из них общежития</t>
+  </si>
+  <si>
+    <t xml:space="preserve">502</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Жилые дома и общежития (сумма строк с 510 по 516, 518, 519)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Использовано
 инвестиций
 в
 фактических
@@ -853,7 +847,7 @@
 рублей</t>
   </si>
   <si>
-    <t>Введено
+    <t xml:space="preserve">Введено
 в
 эксплуатацию
 общей
@@ -862,10 +856,10 @@
 метров</t>
   </si>
   <si>
-    <t>Таблица 9 Строительство жилых домов и общежитий по источникам финансирования</t>
-  </si>
-  <si>
-    <t>Из
+    <t xml:space="preserve">Таблица 9 Строительство жилых домов и общежитий по источникам финансирования</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Из
 них
 в
 сельских
@@ -875,139 +869,139 @@
 метров</t>
   </si>
   <si>
-    <t>четырехкомнатные и более</t>
-  </si>
-  <si>
-    <t>528</t>
-  </si>
-  <si>
-    <t>трехкомнатные</t>
-  </si>
-  <si>
-    <t>527</t>
-  </si>
-  <si>
-    <t>двухкомнатные</t>
-  </si>
-  <si>
-    <t>526</t>
-  </si>
-  <si>
-    <t>в том числе: однокомнатные</t>
-  </si>
-  <si>
-    <t>525</t>
-  </si>
-  <si>
-    <t>Квартиры (сумма строк с 526 по 529)</t>
-  </si>
-  <si>
-    <t>количество,
+    <t xml:space="preserve">четырехкомнатные и более</t>
+  </si>
+  <si>
+    <t xml:space="preserve">528</t>
+  </si>
+  <si>
+    <t xml:space="preserve">трехкомнатные</t>
+  </si>
+  <si>
+    <t xml:space="preserve">527</t>
+  </si>
+  <si>
+    <t xml:space="preserve">двухкомнатные</t>
+  </si>
+  <si>
+    <t xml:space="preserve">526</t>
+  </si>
+  <si>
+    <t xml:space="preserve">в том числе: однокомнатные</t>
+  </si>
+  <si>
+    <t xml:space="preserve">525</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Квартиры (сумма строк с 526 по 529)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">количество,
 единиц</t>
   </si>
   <si>
-    <t>Из них в сельских
+    <t xml:space="preserve">Из них в сельских
 населенных пунктах</t>
   </si>
   <si>
-    <t>Введено в
+    <t xml:space="preserve">Введено в
 эксплуатацию</t>
   </si>
   <si>
-    <t>Таблица 10 Ввод в эксплуатацию квартир в жилых домах</t>
-  </si>
-  <si>
-    <t>общая
+    <t xml:space="preserve">Таблица 10 Ввод в эксплуатацию квартир в жилых домах</t>
+  </si>
+  <si>
+    <t xml:space="preserve">общая
 площадь,
 квадратных
 метров</t>
   </si>
   <si>
-    <t>1027</t>
-  </si>
-  <si>
-    <t>многоквартирные жилые дома</t>
-  </si>
-  <si>
-    <t>1026</t>
-  </si>
-  <si>
-    <t>Из строки 1010: одноквартирные жилые дома</t>
-  </si>
-  <si>
-    <t>1025</t>
-  </si>
-  <si>
-    <t>Общежития</t>
-  </si>
-  <si>
-    <t>1020</t>
-  </si>
-  <si>
-    <t>из других стеновых материалов</t>
-  </si>
-  <si>
-    <t>1019</t>
-  </si>
-  <si>
-    <t>из ячеистого бетона</t>
-  </si>
-  <si>
-    <t>1018</t>
-  </si>
-  <si>
-    <t>из монолитного бетона и монолитного железобетона</t>
-  </si>
-  <si>
-    <t>1017</t>
-  </si>
-  <si>
-    <t>деревянные</t>
-  </si>
-  <si>
-    <t>1016</t>
-  </si>
-  <si>
-    <t>каркасно-блочные</t>
-  </si>
-  <si>
-    <t>1015</t>
-  </si>
-  <si>
-    <t>крупноблочные</t>
-  </si>
-  <si>
-    <t>1014</t>
-  </si>
-  <si>
-    <t>объемно-блочные</t>
-  </si>
-  <si>
-    <t>1013</t>
-  </si>
-  <si>
-    <t>каркасно-панельные</t>
-  </si>
-  <si>
-    <t>1012</t>
-  </si>
-  <si>
-    <t>крупнопанельные</t>
-  </si>
-  <si>
-    <t>1011</t>
-  </si>
-  <si>
-    <t>в том числе: кирпичные</t>
-  </si>
-  <si>
-    <t>1010</t>
-  </si>
-  <si>
-    <t>Жилые дома (без общежитий) - всего (сумма строк с 1011 по 1020)</t>
-  </si>
-  <si>
-    <t>фактическая
+    <t xml:space="preserve">1027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">многоквартирные жилые дома</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Из строки 1010: одноквартирные жилые дома</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Общежития</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">из других стеновых материалов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">из ячеистого бетона</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">из монолитного бетона и монолитного железобетона</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">деревянные</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">каркасно-блочные</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">крупноблочные</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">объемно-блочные</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">каркасно-панельные</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">крупнопанельные</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">в том числе: кирпичные</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Жилые дома (без общежитий) - всего (сумма строк с 1011 по 1020)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">фактическая
 стоимость
 для
 заказчика,
@@ -1015,144 +1009,145 @@
 рублей</t>
   </si>
   <si>
-    <t>введено в
+    <t xml:space="preserve">введено в
 эксплуатацию</t>
   </si>
   <si>
-    <t>Из них в сельских населенных
+    <t xml:space="preserve">Из них в сельских населенных
 пунктах</t>
   </si>
   <si>
-    <t>Таблица 11 Сведения о стоимости строительства жилых домов</t>
-  </si>
-  <si>
-    <t>1036</t>
-  </si>
-  <si>
-    <t>семнадцатиэтажные и более</t>
-  </si>
-  <si>
-    <t>1035</t>
-  </si>
-  <si>
-    <t>десяти-шестнадцатиэтажные</t>
-  </si>
-  <si>
-    <t>1034</t>
-  </si>
-  <si>
-    <t>шести-девятиэтажные</t>
-  </si>
-  <si>
-    <t>1033</t>
-  </si>
-  <si>
-    <t>пятиэтажные</t>
-  </si>
-  <si>
-    <t>1032</t>
-  </si>
-  <si>
-    <t>трех-четырехэтажные</t>
-  </si>
-  <si>
-    <t>1031</t>
-  </si>
-  <si>
-    <t>двухэтажные</t>
-  </si>
-  <si>
-    <t>1030</t>
-  </si>
-  <si>
-    <t>Из суммы строк 1010 и 1025: одноэтажные</t>
-  </si>
-  <si>
-    <t>количество
+    <t xml:space="preserve">Таблица 11 Сведения о стоимости строительства жилых домов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1036</t>
+  </si>
+  <si>
+    <t xml:space="preserve">семнадцатиэтажные и более</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">десяти-шестнадцатиэтажные</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">шести-девятиэтажные</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1033</t>
+  </si>
+  <si>
+    <t xml:space="preserve">пятиэтажные</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1032</t>
+  </si>
+  <si>
+    <t xml:space="preserve">трех-четырехэтажные</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1031</t>
+  </si>
+  <si>
+    <t xml:space="preserve">двухэтажные</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Из суммы строк 1010 и 1025: одноэтажные</t>
+  </si>
+  <si>
+    <t xml:space="preserve">количество
 домов,
 единиц</t>
   </si>
   <si>
-    <t>Таблица 12 Этажность жилых домов и общежитий</t>
-  </si>
-  <si>
-    <t>единиц</t>
-  </si>
-  <si>
-    <t>1061</t>
-  </si>
-  <si>
-    <t>количество квартир (из строки 525)</t>
-  </si>
-  <si>
-    <t>квадратных
+    <t xml:space="preserve">Таблица 12 Этажность жилых домов и общежитий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">единиц</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1061</t>
+  </si>
+  <si>
+    <t xml:space="preserve">количество квартир (из строки 525)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">квадратных
 метров</t>
   </si>
   <si>
-    <t>1060</t>
-  </si>
-  <si>
-    <t>Жилые дома: общая площадь (из строки 502)</t>
-  </si>
-  <si>
-    <t>тысяч
+    <t xml:space="preserve">1060</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Жилые дома: общая площадь (из строки 502)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">тысяч
 рублей</t>
   </si>
   <si>
-    <t>1053</t>
-  </si>
-  <si>
-    <t>1052</t>
-  </si>
-  <si>
-    <t>1051</t>
-  </si>
-  <si>
-    <t>1050</t>
-  </si>
-  <si>
-    <t>Из строки 202 - использовано инвестиций в основной капитал - всего (сумма строк
+    <t xml:space="preserve">1053</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1052</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1051</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1050</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Из строки 202 - использовано инвестиций в основной капитал - всего (сумма строк
 с 1051 по 1053)</t>
   </si>
   <si>
-    <t>Раздел 5</t>
+    <t xml:space="preserve">Раздел 5</t>
   </si>
   <si>
     <t xml:space="preserve">Таблица 13  </t>
   </si>
   <si>
-    <t>Инвестиции в основной капитал и ввод в эксплуатацию жилых домов за счет средств, направленных
+    <t xml:space="preserve">Инвестиции в основной капитал и ввод в эксплуатацию жилых домов за счет средств, направленных
 на преодоление последствий катастрофы на Чернобыльской АЭС</t>
   </si>
   <si>
-    <t>Лицо, ответственное за составление и представление
+    <t xml:space="preserve">Лицо, ответственное за составление и представление
 первичных статистических данных</t>
   </si>
   <si>
-    <t>(должность)</t>
-  </si>
-  <si>
-    <t>(подпись)</t>
-  </si>
-  <si>
-    <t>(инициалы, фамилия)</t>
-  </si>
-  <si>
-    <t>(фамилия, собственное имя, отчество контактного
+    <t xml:space="preserve">(должность)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(подпись)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(инициалы, фамилия)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(фамилия, собственное имя, отчество контактного
 лица, номер телефона, адрес электронной почты)</t>
   </si>
   <si>
-    <t>(дата составления государственной
+    <t xml:space="preserve">(дата составления государственной
 статистической отчетности)</t>
   </si>
   <si>
-    <t>Годовой отчет о вводе в эксплуатацию объектов, основных средств и использовании инвестиций в основной капитал  за</t>
+    <t xml:space="preserve">Годовой отчет о вводе в эксплуатацию объектов, основных средств и использовании инвестиций в основной капитал  за</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="50" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1782,11 +1777,11 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2088,8 +2083,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:M21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A2:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="P10" sqref="P10"/>
@@ -2421,8 +2416,8 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:E22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E22" sqref="C9:E22"/>
@@ -2667,8 +2662,8 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:F14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="C10:F14"/>
@@ -2847,8 +2842,8 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:H24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="H24" sqref="C11:H24"/>
@@ -3209,8 +3204,8 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:F16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="C10:F16"/>
@@ -3413,8 +3408,8 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:J24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A21" sqref="A21:A22"/>
@@ -3657,8 +3652,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10:F10"/>
@@ -3794,8 +3789,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9:E16"/>
@@ -3974,8 +3969,8 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="F33" sqref="C10:F33"/>
@@ -4382,8 +4377,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:C11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C9:C11"/>
@@ -4480,8 +4475,8 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:R13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11:R13"/>
@@ -4868,8 +4863,8 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:F12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="C10:F12"/>
@@ -5027,8 +5022,8 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:H19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
@@ -5309,8 +5304,8 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:E9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>

</xml_diff>